<commit_message>
4. Python Basics for Web Scraping exporting to cvs usinf pandas
</commit_message>
<xml_diff>
--- a/utils/provinces.xlsx
+++ b/utils/provinces.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\src\python\web_scrap\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0306B3DD-847F-49B5-AAC5-1DEA15657C38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD78F4F-602D-4491-AAC8-534018B51285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="7416" windowWidth="23256" windowHeight="12660" xr2:uid="{B0BF5760-A170-4FD2-BEA7-04FF9AA5736B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="133">
   <si>
     <t>Seal</t>
   </si>
@@ -432,6 +432,9 @@
   </si>
   <si>
     <t>KH-</t>
+  </si>
+  <si>
+    <t>,</t>
   </si>
 </sst>
 </file>
@@ -523,7 +526,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -555,6 +558,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -892,8 +896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B95A1B16-A235-41ED-864E-ACEEC325FA62}">
   <dimension ref="A1:AJ26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:AJ1"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2:N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1025,6 +1029,17 @@
       <c r="I2" s="10" t="s">
         <v>13</v>
       </c>
+      <c r="L2" s="11">
+        <f>F2</f>
+        <v>898484</v>
+      </c>
+      <c r="M2" t="s">
+        <v>132</v>
+      </c>
+      <c r="N2" s="11" t="str">
+        <f>L2&amp;M2</f>
+        <v>898484,</v>
+      </c>
     </row>
     <row r="3" spans="1:36" ht="57.75" thickBot="1">
       <c r="A3" s="3"/>
@@ -1052,6 +1067,17 @@
       <c r="I3" s="10" t="s">
         <v>18</v>
       </c>
+      <c r="L3" s="11">
+        <f t="shared" ref="L3:L26" si="0">F3</f>
+        <v>1132017</v>
+      </c>
+      <c r="M3" t="s">
+        <v>132</v>
+      </c>
+      <c r="N3" s="11" t="str">
+        <f t="shared" ref="N3:N26" si="1">L3&amp;M3</f>
+        <v>1132017,</v>
+      </c>
     </row>
     <row r="4" spans="1:36" ht="57.75" thickBot="1">
       <c r="A4" s="3"/>
@@ -1079,6 +1105,17 @@
       <c r="I4" s="10" t="s">
         <v>23</v>
       </c>
+      <c r="L4" s="11">
+        <f t="shared" si="0"/>
+        <v>1062914</v>
+      </c>
+      <c r="M4" t="s">
+        <v>132</v>
+      </c>
+      <c r="N4" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>1062914,</v>
+      </c>
     </row>
     <row r="5" spans="1:36" ht="72" thickBot="1">
       <c r="A5" s="3"/>
@@ -1106,6 +1143,17 @@
       <c r="I5" s="10" t="s">
         <v>28</v>
       </c>
+      <c r="L5" s="11">
+        <f t="shared" si="0"/>
+        <v>604895</v>
+      </c>
+      <c r="M5" t="s">
+        <v>132</v>
+      </c>
+      <c r="N5" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>604895,</v>
+      </c>
     </row>
     <row r="6" spans="1:36" ht="57.75" thickBot="1">
       <c r="A6" s="3"/>
@@ -1133,6 +1181,17 @@
       <c r="I6" s="10" t="s">
         <v>33</v>
       </c>
+      <c r="L6" s="11">
+        <f t="shared" si="0"/>
+        <v>924175</v>
+      </c>
+      <c r="M6" t="s">
+        <v>132</v>
+      </c>
+      <c r="N6" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>924175,</v>
+      </c>
     </row>
     <row r="7" spans="1:36" ht="57.75" thickBot="1">
       <c r="A7" s="3"/>
@@ -1160,6 +1219,17 @@
       <c r="I7" s="10" t="s">
         <v>38</v>
       </c>
+      <c r="L7" s="11">
+        <f t="shared" si="0"/>
+        <v>807254</v>
+      </c>
+      <c r="M7" t="s">
+        <v>132</v>
+      </c>
+      <c r="N7" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>807254,</v>
+      </c>
     </row>
     <row r="8" spans="1:36" ht="43.5" thickBot="1">
       <c r="A8" s="3"/>
@@ -1187,6 +1257,17 @@
       <c r="I8" s="10" t="s">
         <v>43</v>
       </c>
+      <c r="L8" s="11">
+        <f t="shared" si="0"/>
+        <v>682987</v>
+      </c>
+      <c r="M8" t="s">
+        <v>132</v>
+      </c>
+      <c r="N8" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>682987,</v>
+      </c>
     </row>
     <row r="9" spans="1:36" ht="57.75" thickBot="1">
       <c r="A9" s="3"/>
@@ -1214,6 +1295,17 @@
       <c r="I9" s="10" t="s">
         <v>48</v>
       </c>
+      <c r="L9" s="11">
+        <f t="shared" si="0"/>
+        <v>1352198</v>
+      </c>
+      <c r="M9" t="s">
+        <v>132</v>
+      </c>
+      <c r="N9" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>1352198,</v>
+      </c>
     </row>
     <row r="10" spans="1:36" ht="43.5" thickBot="1">
       <c r="A10" s="3"/>
@@ -1241,6 +1333,17 @@
       <c r="I10" s="10" t="s">
         <v>53</v>
       </c>
+      <c r="L10" s="11">
+        <f t="shared" si="0"/>
+        <v>48772</v>
+      </c>
+      <c r="M10" t="s">
+        <v>132</v>
+      </c>
+      <c r="N10" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>48772,</v>
+      </c>
     </row>
     <row r="11" spans="1:36" ht="72" thickBot="1">
       <c r="A11" s="3"/>
@@ -1268,6 +1371,17 @@
       <c r="I11" s="10" t="s">
         <v>58</v>
       </c>
+      <c r="L11" s="11">
+        <f t="shared" si="0"/>
+        <v>140962</v>
+      </c>
+      <c r="M11" t="s">
+        <v>132</v>
+      </c>
+      <c r="N11" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>140962,</v>
+      </c>
     </row>
     <row r="12" spans="1:36" ht="43.5" thickBot="1">
       <c r="A12" s="3"/>
@@ -1295,6 +1409,17 @@
       <c r="I12" s="10" t="s">
         <v>63</v>
       </c>
+      <c r="L12" s="11">
+        <f t="shared" si="0"/>
+        <v>441078</v>
+      </c>
+      <c r="M12" t="s">
+        <v>132</v>
+      </c>
+      <c r="N12" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>441078,</v>
+      </c>
     </row>
     <row r="13" spans="1:36" ht="57.75" thickBot="1">
       <c r="A13" s="3"/>
@@ -1322,6 +1447,17 @@
       <c r="I13" s="10" t="s">
         <v>68</v>
       </c>
+      <c r="L13" s="11">
+        <f t="shared" si="0"/>
+        <v>93657</v>
+      </c>
+      <c r="M13" t="s">
+        <v>132</v>
+      </c>
+      <c r="N13" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>93657,</v>
+      </c>
     </row>
     <row r="14" spans="1:36" ht="57.75" thickBot="1">
       <c r="A14" s="3"/>
@@ -1349,6 +1485,17 @@
       <c r="I14" s="10" t="s">
         <v>73</v>
       </c>
+      <c r="L14" s="11">
+        <f t="shared" si="0"/>
+        <v>267703</v>
+      </c>
+      <c r="M14" t="s">
+        <v>132</v>
+      </c>
+      <c r="N14" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>267703,</v>
+      </c>
     </row>
     <row r="15" spans="1:36" ht="43.5" thickBot="1">
       <c r="A15" s="3"/>
@@ -1376,6 +1523,17 @@
       <c r="I15" s="10" t="s">
         <v>78</v>
       </c>
+      <c r="L15" s="11">
+        <f t="shared" si="0"/>
+        <v>79445</v>
+      </c>
+      <c r="M15" t="s">
+        <v>132</v>
+      </c>
+      <c r="N15" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>79445,</v>
+      </c>
     </row>
     <row r="16" spans="1:36" ht="43.5" thickBot="1">
       <c r="A16" s="3"/>
@@ -1403,8 +1561,19 @@
       <c r="I16" s="10" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="57.75" thickBot="1">
+      <c r="L16" s="11">
+        <f t="shared" si="0"/>
+        <v>2352851</v>
+      </c>
+      <c r="M16" t="s">
+        <v>132</v>
+      </c>
+      <c r="N16" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>2352851,</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="57.75" thickBot="1">
       <c r="A17" s="3"/>
       <c r="B17" s="4" t="s">
         <v>84</v>
@@ -1430,8 +1599,19 @@
       <c r="I17" s="10" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="57.75" thickBot="1">
+      <c r="L17" s="11">
+        <f t="shared" si="0"/>
+        <v>234702</v>
+      </c>
+      <c r="M17" t="s">
+        <v>132</v>
+      </c>
+      <c r="N17" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>234702,</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="57.75" thickBot="1">
       <c r="A18" s="3"/>
       <c r="B18" s="4" t="s">
         <v>89</v>
@@ -1457,8 +1637,19 @@
       <c r="I18" s="10" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" ht="57.75" thickBot="1">
+      <c r="L18" s="11">
+        <f t="shared" si="0"/>
+        <v>249973</v>
+      </c>
+      <c r="M18" t="s">
+        <v>132</v>
+      </c>
+      <c r="N18" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>249973,</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="57.75" thickBot="1">
       <c r="A19" s="3"/>
       <c r="B19" s="4" t="s">
         <v>94</v>
@@ -1484,8 +1675,19 @@
       <c r="I19" s="10" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="43.5" thickBot="1">
+      <c r="L19" s="11">
+        <f t="shared" si="0"/>
+        <v>1277867</v>
+      </c>
+      <c r="M19" t="s">
+        <v>132</v>
+      </c>
+      <c r="N19" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>1277867,</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="43.5" thickBot="1">
       <c r="A20" s="3"/>
       <c r="B20" s="4" t="s">
         <v>99</v>
@@ -1511,8 +1713,19 @@
       <c r="I20" s="10" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" ht="43.5" thickBot="1">
+      <c r="L20" s="11">
+        <f t="shared" si="0"/>
+        <v>516072</v>
+      </c>
+      <c r="M20" t="s">
+        <v>132</v>
+      </c>
+      <c r="N20" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>516072,</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="43.5" thickBot="1">
       <c r="A21" s="3"/>
       <c r="B21" s="4" t="s">
         <v>104</v>
@@ -1538,8 +1751,19 @@
       <c r="I21" s="10" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="57.75" thickBot="1">
+      <c r="L21" s="11">
+        <f t="shared" si="0"/>
+        <v>235852</v>
+      </c>
+      <c r="M21" t="s">
+        <v>132</v>
+      </c>
+      <c r="N21" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>235852,</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="57.75" thickBot="1">
       <c r="A22" s="3"/>
       <c r="B22" s="4" t="s">
         <v>109</v>
@@ -1565,8 +1789,19 @@
       <c r="I22" s="10" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" ht="57.75" thickBot="1">
+      <c r="L22" s="11">
+        <f t="shared" si="0"/>
+        <v>1099825</v>
+      </c>
+      <c r="M22" t="s">
+        <v>132</v>
+      </c>
+      <c r="N22" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>1099825,</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="57.75" thickBot="1">
       <c r="A23" s="3"/>
       <c r="B23" s="4" t="s">
         <v>114</v>
@@ -1592,8 +1827,19 @@
       <c r="I23" s="10" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" ht="57.75" thickBot="1">
+      <c r="L23" s="11">
+        <f t="shared" si="0"/>
+        <v>176488</v>
+      </c>
+      <c r="M23" t="s">
+        <v>132</v>
+      </c>
+      <c r="N23" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>176488,</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="57.75" thickBot="1">
       <c r="A24" s="3"/>
       <c r="B24" s="4" t="s">
         <v>119</v>
@@ -1619,8 +1865,19 @@
       <c r="I24" s="10" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" ht="57.75" thickBot="1">
+      <c r="L24" s="11">
+        <f t="shared" si="0"/>
+        <v>613159</v>
+      </c>
+      <c r="M24" t="s">
+        <v>132</v>
+      </c>
+      <c r="N24" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>613159,</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="57.75" thickBot="1">
       <c r="A25" s="3"/>
       <c r="B25" s="4" t="s">
         <v>124</v>
@@ -1644,8 +1901,19 @@
       <c r="I25" s="10" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" ht="43.5" thickBot="1">
+      <c r="L25" s="11">
+        <f t="shared" si="0"/>
+        <v>1097243</v>
+      </c>
+      <c r="M25" t="s">
+        <v>132</v>
+      </c>
+      <c r="N25" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>1097243,</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="43.5" thickBot="1">
       <c r="A26" s="3"/>
       <c r="B26" s="4" t="s">
         <v>128</v>
@@ -1668,6 +1936,17 @@
       </c>
       <c r="I26" s="10" t="s">
         <v>131</v>
+      </c>
+      <c r="L26" s="11">
+        <f t="shared" si="0"/>
+        <v>889970</v>
+      </c>
+      <c r="M26" t="s">
+        <v>132</v>
+      </c>
+      <c r="N26" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>889970,</v>
       </c>
     </row>
   </sheetData>
@@ -1752,5 +2031,6 @@
     <hyperlink ref="AJ1" r:id="rId78" tooltip="Tboung Khmum province" display="https://en.wikipedia.org/wiki/Tboung_Khmum_province" xr:uid="{C74A610D-B5E6-4C8B-9E34-4A662F6D3B00}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId79"/>
 </worksheet>
 </file>
</xml_diff>